<commit_message>
updates for 2019 and kicad 5
</commit_message>
<xml_diff>
--- a/PCB BOM Template.xlsx
+++ b/PCB BOM Template.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\Documents\GrabCAD\LHRe 2018 Season\18-ELC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\Documents\GrabCAD\LHRe 2019 Season\19-ELC\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5400DA85-6EC9-44F4-8B7F-A3D7F69FD048}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>Refs</t>
   </si>
@@ -45,13 +46,22 @@
   </si>
   <si>
     <t>Footprint</t>
+  </si>
+  <si>
+    <t>19-ELC-1234</t>
+  </si>
+  <si>
+    <t>Mayonnaise Dispenser</t>
+  </si>
+  <si>
+    <t>Longhorn Racing Electric BOM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -62,6 +72,14 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -88,9 +106,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -370,44 +395,80 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" customWidth="1"/>
+    <col min="2" max="2" width="6.28515625" customWidth="1"/>
+    <col min="3" max="7" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+    <row r="1" spans="1:7" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+    </row>
+    <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+    </row>
+    <row r="3" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>6</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B2:D2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
fix template, add requirements.txt
</commit_message>
<xml_diff>
--- a/PCB BOM Template.xlsx
+++ b/PCB BOM Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\Documents\GrabCAD\LHRe 2019 Season\19-ELC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5400DA85-6EC9-44F4-8B7F-A3D7F69FD048}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5EA2E03-E03D-4C51-9FFB-94C85100C13C}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -106,16 +106,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -399,29 +401,29 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" customWidth="1"/>
-    <col min="2" max="2" width="6.28515625" customWidth="1"/>
-    <col min="3" max="7" width="20.5703125" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" style="6" customWidth="1"/>
+    <col min="2" max="2" width="6.28515625" style="6" customWidth="1"/>
+    <col min="3" max="7" width="20.5703125" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -429,9 +431,12 @@
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
     </row>
-    <row r="3" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -439,27 +444,30 @@
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G5" s="3" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>